<commit_message>
Updated verilog to run two cameras simultaneously
Also attempting to add ability to modify pixel offset values, currently
not succeeding. Possibly due to size constraints?
</commit_message>
<xml_diff>
--- a/hardware/datasheets/emcraft_SOM/SOM_pinout.xlsx
+++ b/hardware/datasheets/emcraft_SOM/SOM_pinout.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20475" tabRatio="500" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20475" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="A2F500_FG484" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2496" uniqueCount="1272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2510" uniqueCount="1285">
   <si>
     <t>Pin</t>
   </si>
@@ -3845,6 +3845,45 @@
   </si>
   <si>
     <t>cam0_inphi</t>
+  </si>
+  <si>
+    <t>cam1_resp</t>
+  </si>
+  <si>
+    <t>cam1_incp</t>
+  </si>
+  <si>
+    <t>cam1_cs_n</t>
+  </si>
+  <si>
+    <t>cam1_resv</t>
+  </si>
+  <si>
+    <t>cam1_sdata</t>
+  </si>
+  <si>
+    <t>cam1_incv</t>
+  </si>
+  <si>
+    <t>cam1_sclk</t>
+  </si>
+  <si>
+    <t>cam1_inphi</t>
+  </si>
+  <si>
+    <t>cam1_fifo_afull</t>
+  </si>
+  <si>
+    <t>cam1_frame_capture_done</t>
+  </si>
+  <si>
+    <t>cam1_adc_capture_start</t>
+  </si>
+  <si>
+    <t>cam1_adc_capture_done</t>
+  </si>
+  <si>
+    <t>cam1_fifo_empty</t>
   </si>
 </sst>
 </file>
@@ -15326,8 +15365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G161"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -20178,8 +20217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" topLeftCell="A102" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I125" sqref="I125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -20190,7 +20229,7 @@
     <col min="4" max="4" width="9.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -22239,7 +22278,7 @@
         <v xml:space="preserve">FPGA_GPIO73N </v>
       </c>
       <c r="H68" t="s">
-        <v>1264</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -22302,7 +22341,7 @@
         <v xml:space="preserve">FPGA_GPIO73P </v>
       </c>
       <c r="H70" t="s">
-        <v>1265</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -22425,7 +22464,7 @@
         <v xml:space="preserve">FPGA_GPIO74P </v>
       </c>
       <c r="H74" t="s">
-        <v>1266</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -22458,7 +22497,7 @@
         <v xml:space="preserve">FPGA_GPIO37P </v>
       </c>
       <c r="H75" t="s">
-        <v>1267</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -22551,7 +22590,7 @@
         <v xml:space="preserve">FPGA_GPIO75P </v>
       </c>
       <c r="H78" t="s">
-        <v>1268</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -22584,7 +22623,7 @@
         <v xml:space="preserve">FPGA_GPIO82N </v>
       </c>
       <c r="H79" t="s">
-        <v>1269</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -22617,7 +22656,7 @@
         <v xml:space="preserve">FPGA_GPIO75N </v>
       </c>
       <c r="H80" t="s">
-        <v>1270</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -22650,7 +22689,7 @@
         <v xml:space="preserve">FPGA_GPIO37N </v>
       </c>
       <c r="H81" t="s">
-        <v>1271</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -23103,7 +23142,7 @@
         <v xml:space="preserve">FPGA_GPIO69P </v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" t="str">
         <f>'BSB Headers'!A97</f>
         <v>P11</v>
@@ -23133,7 +23172,7 @@
         <v xml:space="preserve">FPGA_GPIO38P </v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="str">
         <f>'BSB Headers'!A98</f>
         <v>P11</v>
@@ -23163,7 +23202,7 @@
         <v xml:space="preserve">FPGA_GPIO85P </v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="str">
         <f>'BSB Headers'!A99</f>
         <v>P11</v>
@@ -23193,7 +23232,7 @@
         <v xml:space="preserve">FPGA_GPIO38N </v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="str">
         <f>'BSB Headers'!A100</f>
         <v>P11</v>
@@ -23223,7 +23262,7 @@
         <v xml:space="preserve">FPGA_GPIO84N </v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" t="str">
         <f>'BSB Headers'!A101</f>
         <v>P11</v>
@@ -23253,7 +23292,7 @@
         <v xml:space="preserve">FPGA_GPIO36P </v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" t="str">
         <f>'BSB Headers'!A102</f>
         <v>P12</v>
@@ -23283,7 +23322,7 @@
         <v xml:space="preserve">FPGA_GPIO30P </v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" t="str">
         <f>'BSB Headers'!A103</f>
         <v>P12</v>
@@ -23313,7 +23352,7 @@
         <v xml:space="preserve">FPGA_GPIO29N </v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" t="str">
         <f>'BSB Headers'!A104</f>
         <v>P12</v>
@@ -23343,7 +23382,7 @@
         <v xml:space="preserve">FPGA_GPIO30N </v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" t="str">
         <f>'BSB Headers'!A105</f>
         <v>P12</v>
@@ -23373,7 +23412,7 @@
         <v xml:space="preserve">FPGA_GPIO33P </v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" t="str">
         <f>'BSB Headers'!A106</f>
         <v>P12</v>
@@ -23403,7 +23442,7 @@
         <v xml:space="preserve">FPGA_GPIO29P </v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" t="str">
         <f>'BSB Headers'!A107</f>
         <v>P12</v>
@@ -23433,7 +23472,7 @@
         <v xml:space="preserve">FPGA_GPIO33N </v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" t="str">
         <f>'BSB Headers'!A108</f>
         <v>P12</v>
@@ -23462,8 +23501,11 @@
         <f>VLOOKUP($E108, IF($D108="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO31N </v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H108" t="s">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" t="str">
         <f>'BSB Headers'!A109</f>
         <v>P12</v>
@@ -23493,7 +23535,7 @@
         <v xml:space="preserve">FPGA_GPIO28P </v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" t="str">
         <f>'BSB Headers'!A110</f>
         <v>P12</v>
@@ -23522,8 +23564,11 @@
         <f>VLOOKUP($E110, IF($D110="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO31P </v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H110" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" t="str">
         <f>'BSB Headers'!A111</f>
         <v>P12</v>
@@ -23553,7 +23598,7 @@
         <v xml:space="preserve">FPGA_GPIO28N </v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" t="str">
         <f>'BSB Headers'!A112</f>
         <v>P12</v>
@@ -23642,6 +23687,9 @@
         <f>VLOOKUP($E114, IF($D114="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO35P </v>
       </c>
+      <c r="H114" t="s">
+        <v>1266</v>
+      </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" t="str">
@@ -23672,6 +23720,9 @@
         <f>VLOOKUP($E115, IF($D115="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO32N </v>
       </c>
+      <c r="H115" t="s">
+        <v>1267</v>
+      </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" t="str">
@@ -23762,6 +23813,9 @@
         <f>VLOOKUP($E118, IF($D118="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO34P </v>
       </c>
+      <c r="H118" t="s">
+        <v>1268</v>
+      </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" t="str">
@@ -23792,6 +23846,9 @@
         <f>VLOOKUP($E119, IF($D119="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO72P </v>
       </c>
+      <c r="H119" t="s">
+        <v>1269</v>
+      </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" t="str">
@@ -23822,6 +23879,9 @@
         <f>VLOOKUP($E120, IF($D120="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO36N </v>
       </c>
+      <c r="H120" t="s">
+        <v>1270</v>
+      </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" t="str">
@@ -23852,6 +23912,9 @@
         <f>VLOOKUP($E121, IF($D121="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO83P </v>
       </c>
+      <c r="H121" t="s">
+        <v>1271</v>
+      </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" t="str">
@@ -24080,6 +24143,9 @@
         <f>VLOOKUP($E128, IF($D128="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO01P </v>
       </c>
+      <c r="H128" t="s">
+        <v>1280</v>
+      </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" t="str">
@@ -24110,6 +24176,9 @@
         <f>VLOOKUP($E129, IF($D129="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO22N </v>
       </c>
+      <c r="H129" t="s">
+        <v>1281</v>
+      </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" t="str">
@@ -24140,6 +24209,9 @@
         <f>VLOOKUP($E130, IF($D130="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO01N </v>
       </c>
+      <c r="H130" t="s">
+        <v>1282</v>
+      </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" t="str">
@@ -24170,6 +24242,9 @@
         <f>VLOOKUP($E131, IF($D131="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO22P </v>
       </c>
+      <c r="H131" t="s">
+        <v>1283</v>
+      </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" t="str">
@@ -24200,6 +24275,9 @@
         <f>VLOOKUP($E132, IF($D132="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO00P </v>
       </c>
+      <c r="H132" t="s">
+        <v>1284</v>
+      </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="str">
@@ -24229,6 +24307,9 @@
       <c r="G133" t="str">
         <f>VLOOKUP($E133, IF($D133="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO23N </v>
+      </c>
+      <c r="H133" t="s">
+        <v>1263</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated Libero design to include updated verilog files
</commit_message>
<xml_diff>
--- a/hardware/datasheets/emcraft_SOM/SOM_pinout.xlsx
+++ b/hardware/datasheets/emcraft_SOM/SOM_pinout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brghena\workspace\SensEye-2\hardware\datasheets\emcraft_SOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel\Dropbox\lab11\SensEye-2\hardware\datasheets\emcraft_SOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2510" uniqueCount="1285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2512" uniqueCount="1287">
   <si>
     <t>Pin</t>
   </si>
@@ -3884,6 +3884,12 @@
   </si>
   <si>
     <t>cam1_fifo_empty</t>
+  </si>
+  <si>
+    <t>reset</t>
+  </si>
+  <si>
+    <t>clock</t>
   </si>
 </sst>
 </file>
@@ -20217,8 +20223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I125" sqref="I125"/>
+    <sheetView tabSelected="1" topLeftCell="A142" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I164" sqref="I164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -24651,7 +24657,7 @@
         <v xml:space="preserve">MSS_GPIO_12 </v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" t="str">
         <f>'BSB Headers'!A145</f>
         <v>P14</v>
@@ -24681,7 +24687,7 @@
         <v xml:space="preserve">MSS_GPIO_9 </v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" t="str">
         <f>'BSB Headers'!A146</f>
         <v>P14</v>
@@ -24711,7 +24717,7 @@
         <v xml:space="preserve">MSS_GPIO_11 </v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" t="str">
         <f>'BSB Headers'!A147</f>
         <v>P14</v>
@@ -24741,7 +24747,7 @@
         <v xml:space="preserve">MSS_GPIO_8 </v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" t="str">
         <f>'BSB Headers'!A148</f>
         <v>P14</v>
@@ -24771,7 +24777,7 @@
         <v xml:space="preserve">MSS_GPIO_14 </v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" t="str">
         <f>'BSB Headers'!A149</f>
         <v>P14</v>
@@ -24801,7 +24807,7 @@
         <v xml:space="preserve">MSS_GPIO_7 </v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" t="str">
         <f>'BSB Headers'!A150</f>
         <v>P14</v>
@@ -24831,7 +24837,7 @@
         <v xml:space="preserve">MSS_GPIO_15 </v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" t="str">
         <f>'BSB Headers'!A151</f>
         <v>P14</v>
@@ -24861,7 +24867,7 @@
         <v xml:space="preserve">MSS_GPIO_6 </v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" t="str">
         <f>'BSB Headers'!A152</f>
         <v>P14</v>
@@ -24891,7 +24897,7 @@
         <v xml:space="preserve">FPGA_GPIO27P </v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" t="str">
         <f>'BSB Headers'!A153</f>
         <v>P14</v>
@@ -24921,7 +24927,7 @@
         <v xml:space="preserve">MSS_GPIO_5 </v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" t="str">
         <f>'BSB Headers'!A154</f>
         <v>P14</v>
@@ -24951,7 +24957,7 @@
         <v xml:space="preserve">FPGA_GPIO27N </v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" t="str">
         <f>'BSB Headers'!A155</f>
         <v>P14</v>
@@ -24981,7 +24987,7 @@
         <v xml:space="preserve">MSS_GPIO_4 </v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" t="str">
         <f>'BSB Headers'!A156</f>
         <v>P14</v>
@@ -25011,7 +25017,7 @@
         <v xml:space="preserve">FPGA_GPIO26P </v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" t="str">
         <f>'BSB Headers'!A157</f>
         <v>P14</v>
@@ -25041,7 +25047,7 @@
         <v xml:space="preserve">FPGA_GPIO81N </v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" t="str">
         <f>'BSB Headers'!A158</f>
         <v>P14</v>
@@ -25071,7 +25077,7 @@
         <v xml:space="preserve">FPGA_GPIO26N </v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" t="str">
         <f>'BSB Headers'!A159</f>
         <v>P14</v>
@@ -25100,8 +25106,11 @@
         <f>VLOOKUP($E159, IF($D159="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO81P </v>
       </c>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H159" t="s">
+        <v>1285</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" t="str">
         <f>'BSB Headers'!A160</f>
         <v>P14</v>
@@ -25131,7 +25140,7 @@
         <v xml:space="preserve">FPGA_GPIO25P </v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" t="str">
         <f>'BSB Headers'!A161</f>
         <v>P14</v>
@@ -25159,6 +25168,9 @@
       <c r="G161" t="str">
         <f>VLOOKUP($E161, IF($D161="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO84P </v>
+      </c>
+      <c r="H161" t="s">
+        <v>1286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working with 2 cameras
</commit_message>
<xml_diff>
--- a/hardware/datasheets/emcraft_SOM/SOM_pinout.xlsx
+++ b/hardware/datasheets/emcraft_SOM/SOM_pinout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel\Dropbox\lab11\SensEye-2\hardware\datasheets\emcraft_SOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Dropbox\Lab11\SensEye-2\hardware\datasheets\emcraft_SOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
     <sheet name="Connections" sheetId="5" r:id="rId5"/>
     <sheet name="Senseye" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -3895,7 +3895,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -20223,8 +20223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I164" sqref="I164"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L69" sqref="L69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
opencv blob and depth detection working
</commit_message>
<xml_diff>
--- a/hardware/datasheets/emcraft_SOM/SOM_pinout.xlsx
+++ b/hardware/datasheets/emcraft_SOM/SOM_pinout.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2512" uniqueCount="1287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2514" uniqueCount="1287">
   <si>
     <t>Pin</t>
   </si>
@@ -20223,8 +20223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L69" sqref="L69"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H148" sqref="H148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -24533,6 +24533,9 @@
         <f>VLOOKUP($E140, IF($D140="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO71N </v>
       </c>
+      <c r="H140" t="s">
+        <v>1281</v>
+      </c>
       <c r="I140" t="s">
         <v>1255</v>
       </c>
@@ -24565,6 +24568,9 @@
       <c r="G141" t="str">
         <f>VLOOKUP($E141, IF($D141="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO25N </v>
+      </c>
+      <c r="H141" t="s">
+        <v>1259</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated senseye_client to ip addr as input
</commit_message>
<xml_diff>
--- a/hardware/datasheets/emcraft_SOM/SOM_pinout.xlsx
+++ b/hardware/datasheets/emcraft_SOM/SOM_pinout.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2511" uniqueCount="1286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2527" uniqueCount="1302">
   <si>
     <t>Pin</t>
   </si>
@@ -3887,6 +3887,54 @@
   </si>
   <si>
     <t>NOT CONNECTED</t>
+  </si>
+  <si>
+    <t>pupil_loc_h[0]</t>
+  </si>
+  <si>
+    <t>pupil_loc_h[1]</t>
+  </si>
+  <si>
+    <t>pupil_loc_h[2]</t>
+  </si>
+  <si>
+    <t>pupil_loc_h[3]</t>
+  </si>
+  <si>
+    <t>pupil_loc_h[4]</t>
+  </si>
+  <si>
+    <t>pupil_loc_h[5]</t>
+  </si>
+  <si>
+    <t>pupil_loc_h[6]</t>
+  </si>
+  <si>
+    <t>pupil_loc_h[7]</t>
+  </si>
+  <si>
+    <t>pupil_loc_v[0]</t>
+  </si>
+  <si>
+    <t>pupil_loc_v[1]</t>
+  </si>
+  <si>
+    <t>pupil_loc_v[2]</t>
+  </si>
+  <si>
+    <t>pupil_loc_v[3]</t>
+  </si>
+  <si>
+    <t>pupil_loc_v[4]</t>
+  </si>
+  <si>
+    <t>pupil_loc_v[5]</t>
+  </si>
+  <si>
+    <t>pupil_loc_v[6]</t>
+  </si>
+  <si>
+    <t>pupil_loc_v[7]</t>
   </si>
 </sst>
 </file>
@@ -20228,8 +20276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I161"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I95" sqref="I95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -22735,6 +22783,9 @@
         <f>VLOOKUP($E82, IF($D82="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO42P </v>
       </c>
+      <c r="H82" t="s">
+        <v>1286</v>
+      </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="str">
@@ -22765,6 +22816,9 @@
         <f>VLOOKUP($E83, IF($D83="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO41N </v>
       </c>
+      <c r="H83" t="s">
+        <v>1294</v>
+      </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="str">
@@ -22795,6 +22849,9 @@
         <f>VLOOKUP($E84, IF($D84="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO68N </v>
       </c>
+      <c r="H84" t="s">
+        <v>1287</v>
+      </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="str">
@@ -22825,6 +22882,9 @@
         <f>VLOOKUP($E85, IF($D85="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO41P </v>
       </c>
+      <c r="H85" t="s">
+        <v>1295</v>
+      </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="str">
@@ -22855,6 +22915,9 @@
         <f>VLOOKUP($E86, IF($D86="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO68P </v>
       </c>
+      <c r="H86" t="s">
+        <v>1288</v>
+      </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="str">
@@ -22885,6 +22948,9 @@
         <f>VLOOKUP($E87, IF($D87="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO42N </v>
       </c>
+      <c r="H87" t="s">
+        <v>1296</v>
+      </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="str">
@@ -22915,6 +22981,9 @@
         <f>VLOOKUP($E88, IF($D88="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO69N </v>
       </c>
+      <c r="H88" t="s">
+        <v>1289</v>
+      </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="str">
@@ -22945,6 +23014,9 @@
         <f>VLOOKUP($E89, IF($D89="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO40P </v>
       </c>
+      <c r="H89" t="s">
+        <v>1297</v>
+      </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="str">
@@ -22975,6 +23047,9 @@
         <f>VLOOKUP($E90, IF($D90="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO85N </v>
       </c>
+      <c r="H90" t="s">
+        <v>1290</v>
+      </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="str">
@@ -23005,6 +23080,9 @@
         <f>VLOOKUP($E91, IF($D91="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO40N </v>
       </c>
+      <c r="H91" t="s">
+        <v>1298</v>
+      </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="str">
@@ -23035,6 +23113,9 @@
         <f>VLOOKUP($E92, IF($D92="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO70N </v>
       </c>
+      <c r="H92" t="s">
+        <v>1291</v>
+      </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="str">
@@ -23065,6 +23146,9 @@
         <f>VLOOKUP($E93, IF($D93="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO39P </v>
       </c>
+      <c r="H93" t="s">
+        <v>1299</v>
+      </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="str">
@@ -23155,6 +23239,9 @@
         <f>VLOOKUP($E96, IF($D96="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO69P </v>
       </c>
+      <c r="H96" t="s">
+        <v>1292</v>
+      </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" t="str">
@@ -23185,6 +23272,9 @@
         <f>VLOOKUP($E97, IF($D97="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO38P </v>
       </c>
+      <c r="H97" t="s">
+        <v>1300</v>
+      </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="str">
@@ -23215,6 +23305,9 @@
         <f>VLOOKUP($E98, IF($D98="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO85P </v>
       </c>
+      <c r="H98" t="s">
+        <v>1293</v>
+      </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="str">
@@ -23244,6 +23337,9 @@
       <c r="G99" t="str">
         <f>VLOOKUP($E99, IF($D99="P1", 'SOM Board'!$B$2:$F$81, 'SOM Board'!$B$82:$F$161), 2, FALSE)</f>
         <v xml:space="preserve">FPGA_GPIO38N </v>
+      </c>
+      <c r="H99" t="s">
+        <v>1301</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>